<commit_message>
fix sql request 007e1692911e83c4ec07248123ca409ecf27d840
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tlsv-observation.xlsx
+++ b/main/ig/StructureDefinition-tlsv-observation.xlsx
@@ -45,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Observation Telesurveillance</t>
+    <t>Profil Observation pour la telesurveillance</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-21T08:38:54+00:00</t>
+    <t>2024-03-22T13:10:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Update official guide link in implementation guide 19c833dc41b31db717b2fc1a2bd21e0658df9010
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tlsv-observation.xlsx
+++ b/main/ig/StructureDefinition-tlsv-observation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-03T07:57:06+00:00</t>
+    <t>2025-12-03T10:56:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -383,7 +383,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -519,7 +519,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(CarePlan|DeviceRequest|ImmunizationRecommendation|MedicationRequest|NutritionOrder|ServiceRequest)
+    <t xml:space="preserve">Reference(CarePlan|4.0.1|DeviceRequest|4.0.1|ImmunizationRecommendation|4.0.1|MedicationRequest|4.0.1|NutritionOrder|4.0.1|ServiceRequest|4.0.1)
 </t>
   </si>
   <si>
@@ -548,7 +548,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(MedicationAdministration|MedicationDispense|MedicationStatement|Procedure|Immunization|ImagingStudy)
+    <t xml:space="preserve">Reference(MedicationAdministration|4.0.1|MedicationDispense|4.0.1|MedicationStatement|4.0.1|Procedure|4.0.1|Immunization|4.0.1|ImagingStudy|4.0.1)
 </t>
   </si>
   <si>
@@ -662,7 +662,7 @@
     <t>Codes identifying names of simple observations.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes|4.0.1</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -717,7 +717,7 @@
     <t>Observation.focus</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Resource)
+    <t xml:space="preserve">Reference(Resource|4.0.1)
 </t>
   </si>
   <si>
@@ -740,7 +740,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(Encounter|4.0.1)
 </t>
   </si>
   <si>
@@ -831,7 +831,7 @@
     <t>Observation.performer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Practitioner|PractitionerRole|Organization|CareTeam|Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(Practitioner|4.0.1|PractitionerRole|4.0.1|Organization|4.0.1|CareTeam|4.0.1|Patient|4.0.1|RelatedPerson|4.0.1)
 </t>
   </si>
   <si>
@@ -913,7 +913,7 @@
     <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/data-absent-reason</t>
+    <t>http://hl7.org/fhir/ValueSet/data-absent-reason|4.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">obs-6
@@ -945,7 +945,7 @@
     <t>Codes identifying interpretations of observations.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-interpretation</t>
+    <t>http://hl7.org/fhir/ValueSet/observation-interpretation|4.0.1</t>
   </si>
   <si>
     <t>&lt; 260245000 |Findings values|</t>
@@ -1001,7 +1001,7 @@
     <t>Codes describing anatomical locations. May include laterality.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/body-site</t>
+    <t>http://hl7.org/fhir/ValueSet/body-site|4.0.1</t>
   </si>
   <si>
     <t>&lt; 123037004 |Body structure|</t>
@@ -1034,7 +1034,7 @@
     <t>Methods for simple observations.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-methods</t>
+    <t>http://hl7.org/fhir/ValueSet/observation-methods|4.0.1</t>
   </si>
   <si>
     <t>OBX-17</t>
@@ -1046,7 +1046,7 @@
     <t>Observation.specimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Specimen)
+    <t xml:space="preserve">Reference(Specimen|4.0.1)
 </t>
   </si>
   <si>
@@ -1074,7 +1074,7 @@
     <t>Observation.device</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Device|DeviceMetric)
+    <t xml:space="preserve">Reference(Device|4.0.1|DeviceMetric|4.0.1)
 </t>
   </si>
   <si>
@@ -1176,7 +1176,7 @@
     <t>Observation.referenceRange.low</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity {SimpleQuantity}
+    <t xml:space="preserve">Quantity {SimpleQuantity|4.0.1}
 </t>
   </si>
   <si>
@@ -1226,7 +1226,7 @@
     <t>Code for the meaning of a reference range.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/referencerange-meaning</t>
+    <t>http://hl7.org/fhir/ValueSet/referencerange-meaning|4.0.1</t>
   </si>
   <si>
     <t>&lt; 260245000 |Findings values| OR  @@ -1259,7 +1259,7 @@
     <t>Codes identifying the population the reference range applies to.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/referencerange-appliesto</t>
+    <t>http://hl7.org/fhir/ValueSet/referencerange-appliesto|4.0.1</t>
   </si>
   <si>
     <t>Observation.referenceRange.age</t>
@@ -1296,7 +1296,7 @@
     <t>Observation.hasMember</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Observation|QuestionnaireResponse|MolecularSequence)
+    <t xml:space="preserve">Reference(Observation|4.0.1|QuestionnaireResponse|4.0.1|MolecularSequence|4.0.1)
 </t>
   </si>
   <si>
@@ -1746,17 +1746,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="44.67578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="44.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.30078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="38.30078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="34.21875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="111.11328125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="122.43359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1765,28 +1765,28 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="63.70703125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="60.2890625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="41.01953125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="54.6171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="51.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="35.16796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="29.69921875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="247.40625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="25.4609375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="212.10546875" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="107.01953125" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="36.91796875" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="42.34375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="91.75" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="31.65234375" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="36.3046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2997,7 +2997,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
         <v>150</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>190</v>
       </c>
@@ -7951,12 +7951,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AP51">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>